<commit_message>
Bug fix: inoperative 'Export' button.
</commit_message>
<xml_diff>
--- a/nTierApplicationExample/bin/Debug/kisi.xlsx
+++ b/nTierApplicationExample/bin/Debug/kisi.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" r:id="rId1" name="Kisi"/>
-    <sheet sheetId="2" r:id="rId2" name="Sehir"/>
-    <sheet sheetId="3" r:id="rId3" name="Ilce"/>
+    <sheet name="Kisi" sheetId="1" r:id="rId1"/>
+    <sheet name="Sehir" sheetId="2" r:id="rId2"/>
+    <sheet name="Ilce" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" fullCalcOnLoad="true"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>ad</t>
   </si>
@@ -63,9 +63,6 @@
     <t>istanbul</t>
   </si>
   <si>
-    <t>ankara</t>
-  </si>
-  <si>
     <t>e</t>
   </si>
   <si>
@@ -78,12 +75,6 @@
     <t>h</t>
   </si>
   <si>
-    <t>edirne</t>
-  </si>
-  <si>
-    <t>adana</t>
-  </si>
-  <si>
     <t>emrah</t>
   </si>
   <si>
@@ -130,6 +121,12 @@
   </si>
   <si>
     <t>axcv</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>tekirdağ</t>
   </si>
 </sst>
 </file>
@@ -485,10 +482,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2">
         <v>22</v>
@@ -508,22 +505,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D3">
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -531,22 +528,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D4">
         <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -554,22 +551,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D5">
         <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -579,7 +576,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -624,26 +621,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -653,16 +634,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row spans="1:3" outlineLevel="0" r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -673,7 +654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row spans="1:3" outlineLevel="0" r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -684,7 +665,7 @@
         <v>9</v>
       </c>
     </row>
-    <row spans="1:3" outlineLevel="0" r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -695,7 +676,7 @@
         <v>10</v>
       </c>
     </row>
-    <row spans="1:3" outlineLevel="0" r="4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -706,7 +687,7 @@
         <v>11</v>
       </c>
     </row>
-    <row spans="1:3" outlineLevel="0" r="5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -717,7 +698,7 @@
         <v>13</v>
       </c>
     </row>
-    <row spans="1:3" outlineLevel="0" r="6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -725,10 +706,10 @@
         <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row spans="1:3" outlineLevel="0" r="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -736,10 +717,10 @@
         <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row spans="1:3" outlineLevel="0" r="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -747,10 +728,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row spans="1:3" outlineLevel="0" r="9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -758,20 +739,18 @@
         <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2">
         <v>71</v>
       </c>
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
+      <c r="C10" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>